<commit_message>
remove none as a climate choice
</commit_message>
<xml_diff>
--- a/landCoverTemplate.xlsx
+++ b/landCoverTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uq-my.sharepoint.com/personal/uqpscar1_uq_edu_au/Documents/asm/ODK/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2568" documentId="11_D78E0D02123FAFB7EF8F93892FCCBBBD22D96E27" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{622E0841-B363-442C-B907-3C0DBA079537}"/>
+  <xr:revisionPtr revIDLastSave="2570" documentId="11_D78E0D02123FAFB7EF8F93892FCCBBBD22D96E27" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{116AA672-5F6D-4358-94FD-FD35873517FE}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -215,7 +215,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="801" uniqueCount="544">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="544">
   <si>
     <t>type</t>
   </si>
@@ -2179,10 +2179,10 @@
   <dimension ref="A1:AA82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C44" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C67" sqref="C67"/>
+      <selection pane="bottomRight" activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2416,9 +2416,7 @@
       <c r="G12" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="H12" s="3" t="s">
-        <v>434</v>
-      </c>
+      <c r="H12" s="3"/>
     </row>
     <row r="13" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
@@ -3633,13 +3631,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z151"/>
+  <dimension ref="A1:Z150"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C66" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C79" sqref="C79"/>
+      <selection pane="bottomRight" activeCell="A42" sqref="A42:XFD42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4442,11 +4440,11 @@
       <c r="A42" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B42" s="13" t="s">
-        <v>434</v>
+      <c r="B42" s="12" t="s">
+        <v>172</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>435</v>
+        <v>225</v>
       </c>
       <c r="D42" s="3"/>
     </row>
@@ -4455,10 +4453,10 @@
         <v>32</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="D43" s="3"/>
     </row>
@@ -4467,31 +4465,31 @@
         <v>32</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D44" s="3"/>
     </row>
     <row r="45" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B45" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>227</v>
-      </c>
+      <c r="A45" s="6"/>
+      <c r="B45" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="C45" s="6"/>
       <c r="D45" s="3"/>
     </row>
     <row r="46" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="6"/>
-      <c r="B46" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="C46" s="6"/>
+      <c r="A46" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B46" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="D46" s="3"/>
     </row>
     <row r="47" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4499,10 +4497,10 @@
         <v>54</v>
       </c>
       <c r="B47" s="12" t="s">
-        <v>33</v>
+        <v>119</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D47" s="3"/>
     </row>
@@ -4511,10 +4509,10 @@
         <v>54</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>119</v>
+        <v>34</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D48" s="3"/>
     </row>
@@ -4523,34 +4521,33 @@
         <v>54</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>34</v>
+        <v>83</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D49" s="3"/>
     </row>
-    <row r="50" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B50" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="C50" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D50" s="3"/>
+    <row r="51" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="52" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>181</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4558,10 +4555,10 @@
         <v>181</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4569,21 +4566,21 @@
         <v>181</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="B55" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="C55" s="9" t="s">
         <v>189</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="C56" s="9" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4591,10 +4588,10 @@
         <v>194</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4602,10 +4599,10 @@
         <v>194</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4613,10 +4610,10 @@
         <v>194</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>202</v>
+        <v>455</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4624,10 +4621,10 @@
         <v>194</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4635,21 +4632,21 @@
         <v>194</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>456</v>
+        <v>83</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="B62" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="C62" s="9" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="B63" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4657,10 +4654,10 @@
         <v>228</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>232</v>
-      </c>
-      <c r="C64" s="5" t="s">
-        <v>229</v>
+        <v>234</v>
+      </c>
+      <c r="C64" s="9" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4668,10 +4665,10 @@
         <v>228</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4679,21 +4676,21 @@
         <v>228</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>233</v>
+        <v>83</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="B67" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="C67" s="9" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="B68" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4701,10 +4698,10 @@
         <v>255</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4712,10 +4709,10 @@
         <v>255</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4723,10 +4720,10 @@
         <v>255</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4734,10 +4731,10 @@
         <v>255</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>293</v>
+        <v>483</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>261</v>
+        <v>484</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4745,10 +4742,10 @@
         <v>255</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>483</v>
+        <v>289</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>484</v>
+        <v>257</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4756,10 +4753,10 @@
         <v>255</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4767,26 +4764,26 @@
         <v>255</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>290</v>
+        <v>529</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>258</v>
+        <v>530</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="5" t="s">
-        <v>255</v>
-      </c>
       <c r="B76" s="9" t="s">
-        <v>529</v>
-      </c>
-      <c r="C76" s="5" t="s">
-        <v>530</v>
+        <v>102</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="5" t="s">
+        <v>383</v>
+      </c>
       <c r="B77" s="9" t="s">
-        <v>102</v>
+        <v>498</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>497</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4794,10 +4791,10 @@
         <v>383</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>498</v>
+        <v>294</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>497</v>
+        <v>271</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4805,10 +4802,10 @@
         <v>383</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>294</v>
+        <v>386</v>
       </c>
       <c r="C79" s="5" t="s">
-        <v>271</v>
+        <v>387</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4816,10 +4813,10 @@
         <v>383</v>
       </c>
       <c r="B80" s="9" t="s">
-        <v>386</v>
+        <v>295</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>387</v>
+        <v>272</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4827,10 +4824,10 @@
         <v>383</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>295</v>
+        <v>306</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4838,10 +4835,10 @@
         <v>383</v>
       </c>
       <c r="B82" s="9" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>273</v>
+        <v>287</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4849,10 +4846,10 @@
         <v>383</v>
       </c>
       <c r="B83" s="9" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>287</v>
+        <v>274</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4860,10 +4857,10 @@
         <v>383</v>
       </c>
       <c r="B84" s="9" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C84" s="5" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4871,10 +4868,10 @@
         <v>383</v>
       </c>
       <c r="B85" s="9" t="s">
-        <v>298</v>
+        <v>307</v>
       </c>
       <c r="C85" s="5" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4882,10 +4879,10 @@
         <v>383</v>
       </c>
       <c r="B86" s="9" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C86" s="5" t="s">
-        <v>276</v>
+        <v>309</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4893,10 +4890,10 @@
         <v>383</v>
       </c>
       <c r="B87" s="9" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="C87" s="5" t="s">
-        <v>309</v>
+        <v>277</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4904,10 +4901,10 @@
         <v>383</v>
       </c>
       <c r="B88" s="9" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C88" s="5" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4915,10 +4912,10 @@
         <v>383</v>
       </c>
       <c r="B89" s="9" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="C89" s="5" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4926,10 +4923,10 @@
         <v>383</v>
       </c>
       <c r="B90" s="9" t="s">
-        <v>301</v>
+        <v>310</v>
       </c>
       <c r="C90" s="5" t="s">
-        <v>279</v>
+        <v>311</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4937,10 +4934,10 @@
         <v>383</v>
       </c>
       <c r="B91" s="9" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="C91" s="5" t="s">
-        <v>311</v>
+        <v>280</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4948,10 +4945,10 @@
         <v>383</v>
       </c>
       <c r="B92" s="9" t="s">
-        <v>302</v>
+        <v>312</v>
       </c>
       <c r="C92" s="5" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4959,10 +4956,10 @@
         <v>383</v>
       </c>
       <c r="B93" s="9" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C93" s="5" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4970,10 +4967,10 @@
         <v>383</v>
       </c>
       <c r="B94" s="9" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C94" s="5" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4981,10 +4978,10 @@
         <v>383</v>
       </c>
       <c r="B95" s="9" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="C95" s="5" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4992,10 +4989,10 @@
         <v>383</v>
       </c>
       <c r="B96" s="9" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C96" s="5" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5003,10 +5000,10 @@
         <v>383</v>
       </c>
       <c r="B97" s="9" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C97" s="5" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5014,21 +5011,21 @@
         <v>383</v>
       </c>
       <c r="B98" s="9" t="s">
-        <v>305</v>
+        <v>83</v>
       </c>
       <c r="C98" s="5" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="B99" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="C99" s="5" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="B100" s="9" t="s">
+        <v>498</v>
+      </c>
+      <c r="C100" s="5" t="s">
+        <v>497</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5036,10 +5033,10 @@
         <v>384</v>
       </c>
       <c r="B101" s="9" t="s">
-        <v>498</v>
+        <v>347</v>
       </c>
       <c r="C101" s="5" t="s">
-        <v>497</v>
+        <v>319</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5047,10 +5044,10 @@
         <v>384</v>
       </c>
       <c r="B102" s="9" t="s">
-        <v>347</v>
+        <v>352</v>
       </c>
       <c r="C102" s="5" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5058,10 +5055,10 @@
         <v>384</v>
       </c>
       <c r="B103" s="9" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="C103" s="5" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5069,10 +5066,10 @@
         <v>384</v>
       </c>
       <c r="B104" s="9" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="C104" s="5" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5080,10 +5077,10 @@
         <v>384</v>
       </c>
       <c r="B105" s="9" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="C105" s="5" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5091,10 +5088,10 @@
         <v>384</v>
       </c>
       <c r="B106" s="9" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C106" s="5" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5102,10 +5099,10 @@
         <v>384</v>
       </c>
       <c r="B107" s="9" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C107" s="5" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5113,10 +5110,10 @@
         <v>384</v>
       </c>
       <c r="B108" s="9" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C108" s="5" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5124,10 +5121,10 @@
         <v>384</v>
       </c>
       <c r="B109" s="9" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="C109" s="5" t="s">
-        <v>326</v>
+        <v>358</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5135,10 +5132,10 @@
         <v>384</v>
       </c>
       <c r="B110" s="9" t="s">
-        <v>357</v>
+        <v>363</v>
       </c>
       <c r="C110" s="5" t="s">
-        <v>358</v>
+        <v>327</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5146,10 +5143,10 @@
         <v>384</v>
       </c>
       <c r="B111" s="9" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="C111" s="5" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5157,10 +5154,10 @@
         <v>384</v>
       </c>
       <c r="B112" s="9" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="C112" s="5" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5168,10 +5165,10 @@
         <v>384</v>
       </c>
       <c r="B113" s="9" t="s">
-        <v>359</v>
+        <v>350</v>
       </c>
       <c r="C113" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5179,10 +5176,10 @@
         <v>384</v>
       </c>
       <c r="B114" s="9" t="s">
-        <v>350</v>
+        <v>360</v>
       </c>
       <c r="C114" s="5" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5190,10 +5187,10 @@
         <v>384</v>
       </c>
       <c r="B115" s="9" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C115" s="5" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5201,10 +5198,10 @@
         <v>384</v>
       </c>
       <c r="B116" s="9" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C116" s="5" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5212,10 +5209,10 @@
         <v>384</v>
       </c>
       <c r="B117" s="9" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="C117" s="5" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5223,10 +5220,10 @@
         <v>384</v>
       </c>
       <c r="B118" s="9" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="C118" s="5" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5234,10 +5231,10 @@
         <v>384</v>
       </c>
       <c r="B119" s="9" t="s">
-        <v>366</v>
+        <v>385</v>
       </c>
       <c r="C119" s="5" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5245,10 +5242,10 @@
         <v>384</v>
       </c>
       <c r="B120" s="9" t="s">
-        <v>385</v>
+        <v>367</v>
       </c>
       <c r="C120" s="5" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5256,10 +5253,10 @@
         <v>384</v>
       </c>
       <c r="B121" s="9" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C121" s="5" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5267,10 +5264,10 @@
         <v>384</v>
       </c>
       <c r="B122" s="9" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="C122" s="5" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5278,10 +5275,10 @@
         <v>384</v>
       </c>
       <c r="B123" s="9" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="C123" s="5" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="124" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5289,10 +5286,10 @@
         <v>384</v>
       </c>
       <c r="B124" s="9" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="C124" s="5" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5300,10 +5297,10 @@
         <v>384</v>
       </c>
       <c r="B125" s="9" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="C125" s="5" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5311,10 +5308,10 @@
         <v>384</v>
       </c>
       <c r="B126" s="9" t="s">
-        <v>372</v>
+        <v>351</v>
       </c>
       <c r="C126" s="5" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5322,10 +5319,10 @@
         <v>384</v>
       </c>
       <c r="B127" s="9" t="s">
-        <v>351</v>
+        <v>373</v>
       </c>
       <c r="C127" s="5" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5333,10 +5330,10 @@
         <v>384</v>
       </c>
       <c r="B128" s="9" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C128" s="5" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="129" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5344,10 +5341,10 @@
         <v>384</v>
       </c>
       <c r="B129" s="9" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="C129" s="5" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="130" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5355,21 +5352,21 @@
         <v>384</v>
       </c>
       <c r="B130" s="9" t="s">
-        <v>375</v>
+        <v>83</v>
       </c>
       <c r="C130" s="5" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="B131" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="C131" s="5" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="6" t="s">
+        <v>433</v>
+      </c>
+      <c r="B132" s="13" t="s">
+        <v>434</v>
+      </c>
+      <c r="C132" s="6" t="s">
+        <v>435</v>
       </c>
     </row>
     <row r="133" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5377,10 +5374,10 @@
         <v>433</v>
       </c>
       <c r="B133" s="13" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="C133" s="6" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
     </row>
     <row r="134" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5388,10 +5385,10 @@
         <v>433</v>
       </c>
       <c r="B134" s="13" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="C134" s="6" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
     </row>
     <row r="135" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5399,10 +5396,10 @@
         <v>433</v>
       </c>
       <c r="B135" s="13" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="C135" s="6" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
     </row>
     <row r="136" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5410,10 +5407,10 @@
         <v>433</v>
       </c>
       <c r="B136" s="13" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="C136" s="6" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
     </row>
     <row r="137" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5421,10 +5418,10 @@
         <v>433</v>
       </c>
       <c r="B137" s="13" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="C137" s="6" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
     </row>
     <row r="138" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5432,21 +5429,21 @@
         <v>433</v>
       </c>
       <c r="B138" s="13" t="s">
-        <v>444</v>
+        <v>83</v>
       </c>
       <c r="C138" s="6" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="6" t="s">
-        <v>433</v>
-      </c>
-      <c r="B139" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="C139" s="6" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A140" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="B140" s="13" t="s">
+        <v>434</v>
+      </c>
+      <c r="C140" s="6" t="s">
+        <v>435</v>
       </c>
     </row>
     <row r="141" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5454,10 +5451,10 @@
         <v>446</v>
       </c>
       <c r="B141" s="13" t="s">
-        <v>434</v>
+        <v>447</v>
       </c>
       <c r="C141" s="6" t="s">
-        <v>435</v>
+        <v>448</v>
       </c>
     </row>
     <row r="142" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5465,10 +5462,10 @@
         <v>446</v>
       </c>
       <c r="B142" s="13" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="C142" s="6" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
     </row>
     <row r="143" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5476,10 +5473,10 @@
         <v>446</v>
       </c>
       <c r="B143" s="13" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="C143" s="6" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
     </row>
     <row r="144" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5487,10 +5484,10 @@
         <v>446</v>
       </c>
       <c r="B144" s="13" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="C144" s="6" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
     </row>
     <row r="145" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5498,21 +5495,21 @@
         <v>446</v>
       </c>
       <c r="B145" s="13" t="s">
-        <v>453</v>
+        <v>83</v>
       </c>
       <c r="C145" s="6" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="6" t="s">
-        <v>446</v>
-      </c>
-      <c r="B146" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="C146" s="6" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A147" s="5" t="s">
+        <v>461</v>
+      </c>
+      <c r="B147" s="9" t="s">
+        <v>462</v>
+      </c>
+      <c r="C147" s="5" t="s">
+        <v>479</v>
       </c>
     </row>
     <row r="148" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5520,10 +5517,10 @@
         <v>461</v>
       </c>
       <c r="B148" s="9" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="C148" s="5" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
     </row>
     <row r="149" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5531,10 +5528,10 @@
         <v>461</v>
       </c>
       <c r="B149" s="9" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="C149" s="5" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
     </row>
     <row r="150" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5542,20 +5539,9 @@
         <v>461</v>
       </c>
       <c r="B150" s="9" t="s">
-        <v>464</v>
+        <v>83</v>
       </c>
       <c r="C150" s="5" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="151" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="5" t="s">
-        <v>461</v>
-      </c>
-      <c r="B151" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="C151" s="5" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>